<commit_message>
Small change to screws
Modified them to 2.2mm in diameter. Seems the fab house changed them from 3mm to 2.2mm in the order, which actually worked out better for fitting screws in.

The 'top-left' screw (between pin header and ICSP header) was moved 0.3mm to the right to allow more of the ground plane to connect. Will be reflected in the 3D model of the casing.
</commit_message>
<xml_diff>
--- a/L-COM system (name subject to change)/Parts.xlsx
+++ b/L-COM system (name subject to change)/Parts.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="216">
   <si>
     <t>Part type:</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Male-male Molex Mini-Lock connectors (individual parts)</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/61200621621/4846913</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC152LFBN-RC/810221</t>
   </si>
   <si>
@@ -577,9 +574,6 @@
     <t>Clock source</t>
   </si>
   <si>
-    <t>TOO BIG</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/molex/0732511150/1465156</t>
   </si>
   <si>
@@ -671,6 +665,15 @@
   </si>
   <si>
     <t>1206 (3216)</t>
+  </si>
+  <si>
+    <t>4x M2 screws</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/amphenol-icc-fci/69168-106HLF/1002738</t>
+  </si>
+  <si>
+    <t>TEST PART</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -950,6 +953,8 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
@@ -1239,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O35"/>
+  <dimension ref="A2:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>41</v>
@@ -1352,13 +1357,13 @@
         <v>55</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>56</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1372,7 +1377,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>42</v>
@@ -1425,7 +1430,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>100</v>
@@ -1457,7 +1462,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I8" s="17"/>
       <c r="K8" s="13" t="s">
@@ -1523,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I10" s="17"/>
       <c r="K10" s="7" t="s">
@@ -1564,10 +1569,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>40</v>
@@ -1675,7 +1680,7 @@
         <v>11</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N15" s="17"/>
     </row>
@@ -1707,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N16" s="17"/>
     </row>
@@ -1748,10 +1753,10 @@
         <v>37</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>40</v>
@@ -1865,7 +1870,7 @@
       <c r="M25" s="22"/>
       <c r="N25" s="17"/>
       <c r="O25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1893,7 +1898,7 @@
       </c>
       <c r="M26" s="19"/>
       <c r="N26" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1960,7 +1965,7 @@
         <v>11</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="21"/>
@@ -1989,10 +1994,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="17"/>
@@ -2006,6 +2011,11 @@
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="18"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2016,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2063,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="9"/>
       <c r="G2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2076,7 +2086,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2090,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="26">
         <v>0.2</v>
@@ -2108,7 +2118,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="26">
         <v>0.2</v>
@@ -2126,13 +2136,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6" s="26">
         <v>0.21</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2146,7 +2156,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="26">
         <v>0.19</v>
@@ -2164,30 +2174,30 @@
         <v>2</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E8" s="26">
         <v>0.38</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G8" t="s">
         <v>199</v>
-      </c>
-      <c r="G8" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" s="32">
         <v>2</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E9" s="27">
         <v>0.92</v>
@@ -2198,10 +2208,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2224,7 +2234,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="9"/>
       <c r="G13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2247,7 +2257,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,7 +2271,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" s="26">
         <v>0.15</v>
@@ -2270,7 +2280,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>11</v>
@@ -2279,7 +2289,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="26">
         <v>0.15</v>
@@ -2297,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="26">
         <v>0.15</v>
@@ -2315,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E18" s="26">
         <v>0.15</v>
@@ -2333,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" s="26">
         <v>0.15</v>
@@ -2351,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E20" s="26">
         <v>0.15</v>
@@ -2360,7 +2370,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>11</v>
@@ -2369,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E21" s="27">
         <v>1.62</v>
@@ -2421,7 +2431,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C26" s="32">
         <v>1</v>
@@ -2512,18 +2522,18 @@
       </c>
       <c r="F32" s="18"/>
       <c r="H32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C33" s="28"/>
       <c r="E33" s="23"/>
       <c r="H33" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I33" s="37"/>
       <c r="K33" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L33" s="37"/>
     </row>
@@ -2531,16 +2541,16 @@
       <c r="C34" s="28"/>
       <c r="E34" s="23"/>
       <c r="H34" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I34" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="K34" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="K34" s="36" t="s">
-        <v>158</v>
-      </c>
       <c r="L34" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2594,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E37" s="26">
         <v>0.26</v>
@@ -2613,12 +2623,12 @@
         <v>72</v>
       </c>
       <c r="M37" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>11</v>
@@ -2627,7 +2637,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="27">
         <v>0.26</v>
@@ -2646,7 +2656,7 @@
         <v>72</v>
       </c>
       <c r="M38" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2718,10 +2728,10 @@
         <v>12.85</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2743,10 +2753,10 @@
         <v>0.88</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -2811,7 +2821,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>11</v>
@@ -2820,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E49" s="27">
         <v>0.71</v>
@@ -2835,10 +2845,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>174</v>
       </c>
       <c r="E50" s="23"/>
       <c r="H50" s="2"/>
@@ -2920,7 +2930,7 @@
         <v>39.6</v>
       </c>
       <c r="M54" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -2951,7 +2961,7 @@
         <v>16.5</v>
       </c>
       <c r="M55" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -3010,14 +3020,14 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B60" s="43"/>
       <c r="C60" s="31">
         <v>1</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E60" s="26">
         <v>0.49</v>
@@ -3056,10 +3066,10 @@
         <v>3750</v>
       </c>
       <c r="M61" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -3129,13 +3139,13 @@
         <v>1</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>132</v>
+        <v>214</v>
       </c>
       <c r="E66" s="26">
         <v>0.65</v>
       </c>
-      <c r="F66" s="17" t="s">
-        <v>183</v>
+      <c r="F66" s="45" t="s">
+        <v>215</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -3197,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E69" s="26">
         <v>2.63</v>
@@ -3219,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E70" s="27">
         <v>4.97</v>
@@ -3232,10 +3242,10 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>185</v>
-      </c>
-      <c r="B71" t="s">
-        <v>186</v>
+        <v>183</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>184</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -3244,7 +3254,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -3276,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C76" s="29"/>
       <c r="D76" s="11"/>
@@ -3292,13 +3302,13 @@
         <v>62</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C77" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E77" s="25" t="s">
         <v>12</v>
@@ -3313,22 +3323,22 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C78" s="32">
         <v>1</v>
       </c>
       <c r="D78" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E78" s="27">
         <v>8.07</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3354,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C81" s="29"/>
       <c r="D81" s="11"/>
@@ -3370,13 +3380,13 @@
         <v>62</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C82" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E82" s="25" t="s">
         <v>12</v>
@@ -3419,16 +3429,16 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H85" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="I85" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="I85" s="36" t="s">
-        <v>171</v>
-      </c>
       <c r="K85" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="L85" s="36" t="s">
         <v>170</v>
-      </c>
-      <c r="L85" s="36" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3650,26 +3660,26 @@
     <hyperlink ref="D26" r:id="rId14"/>
     <hyperlink ref="D70" r:id="rId15"/>
     <hyperlink ref="D69" r:id="rId16"/>
-    <hyperlink ref="D66" r:id="rId17"/>
-    <hyperlink ref="D78" r:id="rId18"/>
-    <hyperlink ref="D103" r:id="rId19"/>
-    <hyperlink ref="D102" r:id="rId20"/>
-    <hyperlink ref="D38" r:id="rId21"/>
-    <hyperlink ref="D37" r:id="rId22"/>
-    <hyperlink ref="D20" r:id="rId23"/>
-    <hyperlink ref="D19" r:id="rId24"/>
+    <hyperlink ref="D78" r:id="rId17"/>
+    <hyperlink ref="D103" r:id="rId18"/>
+    <hyperlink ref="D102" r:id="rId19"/>
+    <hyperlink ref="D38" r:id="rId20"/>
+    <hyperlink ref="D37" r:id="rId21"/>
+    <hyperlink ref="D20" r:id="rId22"/>
+    <hyperlink ref="D19" r:id="rId23"/>
     <hyperlink ref="D18" display="https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805JT1K80/1757793?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRAGYBOcgJkpAF0CAHAFyhAGVWAnASwB2AcxABfAmDoRoIZJHTZ8RUhWo0AHIxbtIXXoJHjwldfRlyFuAsUhkADFpBsO3fsLEEad9QFYEs1EwrZVtwADp1AAIAawB5AA"/>
-    <hyperlink ref="D17" r:id="rId25"/>
-    <hyperlink ref="D16" r:id="rId26"/>
+    <hyperlink ref="D17" r:id="rId24"/>
+    <hyperlink ref="D16" r:id="rId25"/>
     <hyperlink ref="D15" display="https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805ZT0R00/1756901?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvjAA2eCCSQ0WPIRIgAzDRUw6jEK3Zc%2BQ0eM0RoMlBhz4ikUmo0UGzNpE48BwseBoU6Z2fJWSrYgZE46Lm4Gnvgwl"/>
-    <hyperlink ref="D9" r:id="rId27"/>
-    <hyperlink ref="D8" r:id="rId28"/>
-    <hyperlink ref="D7" r:id="rId29"/>
-    <hyperlink ref="D6" r:id="rId30"/>
-    <hyperlink ref="D5" r:id="rId31"/>
-    <hyperlink ref="D4" r:id="rId32"/>
-    <hyperlink ref="D49" r:id="rId33"/>
-    <hyperlink ref="D21" r:id="rId34"/>
+    <hyperlink ref="D9" r:id="rId26"/>
+    <hyperlink ref="D8" r:id="rId27"/>
+    <hyperlink ref="D7" r:id="rId28"/>
+    <hyperlink ref="D6" r:id="rId29"/>
+    <hyperlink ref="D5" r:id="rId30"/>
+    <hyperlink ref="D4" r:id="rId31"/>
+    <hyperlink ref="D49" r:id="rId32"/>
+    <hyperlink ref="D21" r:id="rId33"/>
+    <hyperlink ref="B71" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>
@@ -3688,7 +3698,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -3696,12 +3706,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -3709,22 +3719,22 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
@@ -3732,17 +3742,17 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
@@ -3750,7 +3760,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>